<commit_message>
Updated optimization workflow. Need to write script to work with papermill
</commit_message>
<xml_diff>
--- a/case_studies/borrowing_hydrogen/inputs/reactions.xlsx
+++ b/case_studies/borrowing_hydrogen/inputs/reactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kobi/Documents/Research/summit/case_studies/borrowing_hydrogen/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD345A6F-98AB-7F49-8E61-35C95E9A7053}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2323404-4EB3-9247-8E12-6450314271EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23480" yWindow="6060" windowWidth="19640" windowHeight="15540" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -23,8 +23,8 @@
     <sheet name="42-ethylbenzene" sheetId="12" r:id="rId8"/>
     <sheet name="43-butanol" sheetId="13" r:id="rId9"/>
     <sheet name="44-pyridine" sheetId="10" r:id="rId10"/>
-    <sheet name="44-toluene" sheetId="14" r:id="rId11"/>
-    <sheet name="45-acetic-acid" sheetId="15" r:id="rId12"/>
+    <sheet name="45-dmso" sheetId="14" r:id="rId11"/>
+    <sheet name="46-toluene" sheetId="15" r:id="rId12"/>
     <sheet name="46-heptane" sheetId="16" r:id="rId13"/>
     <sheet name="47-oxane" sheetId="17" r:id="rId14"/>
     <sheet name="48-propanitirle" sheetId="18" r:id="rId15"/>
@@ -37,9 +37,9 @@
     <definedName name="_xlnm.Print_Area" localSheetId="7">'42-ethylbenzene'!$A$1:$N$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="8">'43-butanol'!$A$1:$N$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="9">'44-pyridine'!$A$1:$N$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="10">'44-toluene'!$A$1:$N$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="11">'45-acetic-acid'!$A$1:$N$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">'45-dmso'!$A$1:$N$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="12">'46-heptane'!$A$1:$N$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="11">'46-toluene'!$A$1:$N$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="13">'47-oxane'!$A$1:$N$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="14">'48-propanitirle'!$A$1:$N$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Template!$A$1:$N$15</definedName>
@@ -1699,21 +1699,30 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>O Zhurakovskyi:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Automatic.</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>O Zhurakovskyi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Automatic.</t>
         </r>
       </text>
     </comment>
@@ -8161,12 +8170,6 @@
     <t>toluene                   (CAS: 108-88-3)</t>
   </si>
   <si>
-    <t>msc H2O, EtOH, eth, ace, bz; s chl, CS2l;  bp 117°C</t>
-  </si>
-  <si>
-    <t>acetic acid              (CAS: 64-19-7)</t>
-  </si>
-  <si>
     <t>heptane                  (CAS: 142-82-5)</t>
   </si>
   <si>
@@ -8202,6 +8205,12 @@
   <si>
     <t>1-butanol                (CAS: 71-36-3)</t>
   </si>
+  <si>
+    <t>s H2O, EtOH, eth, ace, ctc, AcOEt;     bp 191°C</t>
+  </si>
+  <si>
+    <t>dimethyl sulfoxide                   (CAS: 67-68-5)</t>
+  </si>
 </sst>
 </file>
 
@@ -8210,7 +8219,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8316,6 +8325,22 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -8337,7 +8362,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -8637,12 +8662,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -8858,6 +8922,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8897,15 +8997,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -8924,29 +9015,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10262,55 +10407,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="107" t="str">
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
         <v>BH-Template</v>
       </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="108"/>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -10340,11 +10485,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -10388,11 +10533,11 @@
       <c r="K5" s="67">
         <v>1</v>
       </c>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -10433,11 +10578,11 @@
       </c>
       <c r="J6" s="63"/>
       <c r="K6" s="68"/>
-      <c r="L6" s="96" t="s">
+      <c r="L6" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="96"/>
-      <c r="N6" s="97"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="109"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -10472,11 +10617,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -10517,9 +10662,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -10550,9 +10695,9 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
@@ -10569,19 +10714,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="93">
+      <c r="I10" s="105">
         <f>I5/(SUM(D10:D12))</f>
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="102" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="26"/>
-      <c r="L10" s="101" t="s">
+      <c r="L10" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
@@ -10596,8 +10741,8 @@
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="103"/>
       <c r="K11" s="12"/>
       <c r="L11" s="51"/>
       <c r="M11" s="51"/>
@@ -10616,12 +10761,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -10649,9 +10794,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -10690,9 +10835,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -10700,12 +10845,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="J1:L1"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="L13:N13"/>
     <mergeCell ref="A2:N3"/>
@@ -10716,6 +10855,12 @@
     <mergeCell ref="L10:N10"/>
     <mergeCell ref="L12:N12"/>
     <mergeCell ref="L8:N8"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -10749,8 +10894,8 @@
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N3"/>
+    <sheetView zoomScale="117" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10772,55 +10917,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="107" t="str">
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
         <v>BH-44-pyridine</v>
       </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" s="108"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -10850,11 +10995,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -10894,11 +11039,11 @@
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="67"/>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -10941,11 +11086,11 @@
         <v>1.0129999999999999</v>
       </c>
       <c r="K6" s="82"/>
-      <c r="L6" s="98" t="s">
+      <c r="L6" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="99"/>
-      <c r="N6" s="100"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="93"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -10980,11 +11125,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -11019,9 +11164,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -11052,9 +11197,9 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
@@ -11071,19 +11216,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="93">
+      <c r="I10" s="105">
         <f>I5/(SUM(D10:D12))</f>
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="102" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="78"/>
-      <c r="L10" s="101" t="s">
+      <c r="L10" s="110" t="s">
         <v>55</v>
       </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
@@ -11094,12 +11239,12 @@
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="103"/>
       <c r="K11" s="31"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
-      <c r="N11" s="106"/>
+      <c r="L11" s="114"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="115"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
@@ -11114,12 +11259,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -11147,9 +11292,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -11188,9 +11333,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -11198,11 +11343,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
     <mergeCell ref="L6:N6"/>
     <mergeCell ref="L11:N11"/>
     <mergeCell ref="L5:N5"/>
@@ -11215,6 +11355,11 @@
     <mergeCell ref="J10:J12"/>
     <mergeCell ref="L10:N10"/>
     <mergeCell ref="L12:N12"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -11248,8 +11393,8 @@
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11271,55 +11416,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="107" t="str">
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
-        <v>BH-44-toluene</v>
-      </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+        <v>BH-45-dmso</v>
+      </c>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" s="108"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -11349,11 +11494,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -11393,11 +11538,11 @@
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="67"/>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -11440,11 +11585,11 @@
         <v>1.0129999999999999</v>
       </c>
       <c r="K6" s="82"/>
-      <c r="L6" s="98" t="s">
+      <c r="L6" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="99"/>
-      <c r="N6" s="100"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="93"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -11479,11 +11624,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -11518,9 +11663,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -11551,14 +11696,14 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
       <c r="B10" s="84" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="65">
@@ -11570,19 +11715,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="93">
+      <c r="I10" s="105">
         <f>I5/(SUM(D10:D12))</f>
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="80"/>
-      <c r="L10" s="101" t="s">
-        <v>58</v>
-      </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="K10" s="85"/>
+      <c r="L10" s="110" t="s">
+        <v>72</v>
+      </c>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
@@ -11593,12 +11738,12 @@
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="103"/>
       <c r="K11" s="31"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
-      <c r="N11" s="106"/>
+      <c r="L11" s="114"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="115"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
@@ -11613,12 +11758,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -11646,9 +11791,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -11687,9 +11832,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -11697,23 +11842,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L12:N12"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A2:N3"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -11747,8 +11892,8 @@
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11770,55 +11915,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="107" t="str">
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
-        <v>BH-45-acetic-acid</v>
-      </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+        <v>BH-46-toluene</v>
+      </c>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="108"/>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -11848,11 +11993,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -11892,11 +12037,11 @@
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="67"/>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -11939,11 +12084,11 @@
         <v>1.0129999999999999</v>
       </c>
       <c r="K6" s="82"/>
-      <c r="L6" s="98" t="s">
+      <c r="L6" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="99"/>
-      <c r="N6" s="100"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="93"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -11978,11 +12123,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -12017,9 +12162,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -12050,74 +12195,73 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
-      <c r="B10" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="65">
+      <c r="B10" s="116" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="117"/>
+      <c r="D10" s="118">
         <v>5</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="93">
-        <f>I5/(SUM(D10:D12))</f>
+      <c r="F10" s="117"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="117"/>
+      <c r="I10" s="130">
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="80"/>
-      <c r="L10" s="101" t="s">
-        <v>60</v>
-      </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="136" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" s="136"/>
+      <c r="N10" s="137"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
-      <c r="N11" s="106"/>
+      <c r="B11" s="121"/>
+      <c r="C11" s="122"/>
+      <c r="D11" s="123"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="124"/>
+      <c r="H11" s="122"/>
+      <c r="I11" s="131"/>
+      <c r="J11" s="134"/>
+      <c r="K11" s="121"/>
+      <c r="L11" s="138"/>
+      <c r="M11" s="138"/>
+      <c r="N11" s="139"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="66">
+      <c r="B12" s="125"/>
+      <c r="C12" s="126"/>
+      <c r="D12" s="127">
         <v>0</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="F12" s="128"/>
+      <c r="G12" s="128"/>
+      <c r="H12" s="126"/>
+      <c r="I12" s="132"/>
+      <c r="J12" s="135"/>
+      <c r="K12" s="129"/>
+      <c r="L12" s="140"/>
+      <c r="M12" s="140"/>
+      <c r="N12" s="141"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -12145,9 +12289,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -12186,9 +12330,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -12196,23 +12340,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L12:N12"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A2:N3"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -12231,7 +12375,7 @@
           <x14:formula1>
             <xm:f>Settings!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E10:E12 G5:G10</xm:sqref>
+          <xm:sqref>G5:G9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -12269,55 +12413,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="107" t="str">
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
         <v>BH-46-heptane</v>
       </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="108"/>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -12347,11 +12491,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -12391,11 +12535,11 @@
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="67"/>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -12438,11 +12582,11 @@
         <v>1.0129999999999999</v>
       </c>
       <c r="K6" s="82"/>
-      <c r="L6" s="98" t="s">
+      <c r="L6" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="99"/>
-      <c r="N6" s="100"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="93"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -12477,11 +12621,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -12516,9 +12660,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -12549,14 +12693,14 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
       <c r="B10" s="84" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="65">
@@ -12568,19 +12712,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="93">
+      <c r="I10" s="105">
         <f>I5/(SUM(D10:D12))</f>
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="102" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="80"/>
-      <c r="L10" s="101" t="s">
-        <v>63</v>
-      </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="L10" s="110" t="s">
+        <v>61</v>
+      </c>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
@@ -12591,12 +12735,12 @@
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="103"/>
       <c r="K11" s="31"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
-      <c r="N11" s="106"/>
+      <c r="L11" s="114"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="115"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
@@ -12611,12 +12755,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -12644,9 +12788,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -12685,9 +12829,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -12695,23 +12839,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L12:N12"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A2:N3"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -12769,57 +12913,57 @@
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="107" t="str">
+        <v>64</v>
+      </c>
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
         <v>BH-47-oxane</v>
       </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="108"/>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -12849,11 +12993,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -12893,11 +13037,11 @@
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="67"/>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -12940,11 +13084,11 @@
         <v>1.0129999999999999</v>
       </c>
       <c r="K6" s="82"/>
-      <c r="L6" s="98" t="s">
+      <c r="L6" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="99"/>
-      <c r="N6" s="100"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="93"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -12979,11 +13123,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -13018,9 +13162,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -13051,14 +13195,14 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
       <c r="B10" s="84" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="65">
@@ -13070,19 +13214,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="93">
+      <c r="I10" s="105">
         <f>I5/(SUM(D10:D12))</f>
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="102" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="80"/>
-      <c r="L10" s="101" t="s">
-        <v>67</v>
-      </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="L10" s="110" t="s">
+        <v>65</v>
+      </c>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
@@ -13093,12 +13237,12 @@
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="103"/>
       <c r="K11" s="31"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
-      <c r="N11" s="106"/>
+      <c r="L11" s="114"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="115"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
@@ -13113,12 +13257,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -13146,9 +13290,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -13187,9 +13331,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -13197,23 +13341,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L12:N12"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A2:N3"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -13270,55 +13414,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="107" t="str">
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
         <v>BH-48-propanitirle</v>
       </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="108"/>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -13348,11 +13492,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -13392,11 +13536,11 @@
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="67"/>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -13439,11 +13583,11 @@
         <v>1.0129999999999999</v>
       </c>
       <c r="K6" s="82"/>
-      <c r="L6" s="98" t="s">
+      <c r="L6" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="99"/>
-      <c r="N6" s="100"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="93"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -13478,11 +13622,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -13517,9 +13661,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -13550,14 +13694,14 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
       <c r="B10" s="84" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="65">
@@ -13569,19 +13713,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="93">
+      <c r="I10" s="105">
         <f>I5/(SUM(D10:D12))</f>
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="102" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="80"/>
-      <c r="L10" s="101" t="s">
-        <v>64</v>
-      </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="L10" s="110" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
@@ -13592,12 +13736,12 @@
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="103"/>
       <c r="K11" s="31"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
-      <c r="N11" s="106"/>
+      <c r="L11" s="114"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="115"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
@@ -13612,12 +13756,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -13645,9 +13789,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -13686,9 +13830,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -13696,23 +13840,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L12:N12"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A2:N3"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -13957,55 +14101,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="107" t="str">
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
         <v>BH-36-Toluene</v>
       </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="108"/>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -14035,11 +14179,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -14083,11 +14227,11 @@
       <c r="K5" s="67">
         <v>1</v>
       </c>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -14128,11 +14272,11 @@
       </c>
       <c r="J6" s="63"/>
       <c r="K6" s="68"/>
-      <c r="L6" s="96" t="s">
+      <c r="L6" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="96"/>
-      <c r="N6" s="97"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="109"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -14167,11 +14311,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -14206,9 +14350,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -14239,9 +14383,9 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
@@ -14258,19 +14402,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="93">
+      <c r="I10" s="105">
         <f>I5/(SUM(D10:D12))</f>
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="102" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="44"/>
-      <c r="L10" s="101" t="s">
+      <c r="L10" s="110" t="s">
         <v>58</v>
       </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
@@ -14285,8 +14429,8 @@
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="103"/>
       <c r="K11" s="12"/>
       <c r="L11" s="51"/>
       <c r="M11" s="51"/>
@@ -14305,12 +14449,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -14338,9 +14482,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -14379,9 +14523,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -14389,6 +14533,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="J10:J12"/>
     <mergeCell ref="L10:N10"/>
@@ -14399,12 +14549,6 @@
     <mergeCell ref="A2:N3"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -14461,55 +14605,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="107" t="str">
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
         <v>BH-37-sulfolane</v>
       </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="108"/>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -14539,11 +14683,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -14587,11 +14731,11 @@
       <c r="K5" s="67">
         <v>1</v>
       </c>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -14632,11 +14776,11 @@
       </c>
       <c r="J6" s="63"/>
       <c r="K6" s="68"/>
-      <c r="L6" s="96" t="s">
+      <c r="L6" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="96"/>
-      <c r="N6" s="97"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="109"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -14671,11 +14815,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -14710,9 +14854,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -14743,9 +14887,9 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
@@ -14762,19 +14906,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="93">
+      <c r="I10" s="105">
         <f>I5/(SUM(D10:D12))</f>
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="102" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="44"/>
-      <c r="L10" s="101" t="s">
+      <c r="L10" s="110" t="s">
         <v>49</v>
       </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
@@ -14789,8 +14933,8 @@
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="103"/>
       <c r="K11" s="12"/>
       <c r="L11" s="51"/>
       <c r="M11" s="51"/>
@@ -14809,12 +14953,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -14842,9 +14986,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -14883,9 +15027,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -14893,6 +15037,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="J10:J12"/>
     <mergeCell ref="L10:N10"/>
@@ -14903,12 +15053,6 @@
     <mergeCell ref="A2:N3"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -14965,55 +15109,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="107" t="str">
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
         <v>BH-38-nitromethane</v>
       </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="108"/>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -15043,11 +15187,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -15091,11 +15235,11 @@
       <c r="K5" s="67">
         <v>1</v>
       </c>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -15136,11 +15280,11 @@
       </c>
       <c r="J6" s="63"/>
       <c r="K6" s="68"/>
-      <c r="L6" s="96" t="s">
+      <c r="L6" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="96"/>
-      <c r="N6" s="97"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="109"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -15175,11 +15319,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -15214,9 +15358,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -15247,9 +15391,9 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
@@ -15266,19 +15410,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="93">
+      <c r="I10" s="105">
         <f>I5/(SUM(D10:D12))</f>
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="102" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="44"/>
-      <c r="L10" s="101" t="s">
+      <c r="L10" s="110" t="s">
         <v>51</v>
       </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
@@ -15293,8 +15437,8 @@
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="103"/>
       <c r="K11" s="12"/>
       <c r="L11" s="51"/>
       <c r="M11" s="51"/>
@@ -15313,12 +15457,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -15346,9 +15490,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -15387,9 +15531,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -15397,6 +15541,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="J10:J12"/>
     <mergeCell ref="L10:N10"/>
@@ -15407,12 +15557,6 @@
     <mergeCell ref="A2:N3"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -15469,55 +15613,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="107" t="str">
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
         <v>BH-38-dimethyl acetamide</v>
       </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="108"/>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -15547,11 +15691,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -15595,11 +15739,11 @@
       <c r="K5" s="67">
         <v>1</v>
       </c>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -15640,11 +15784,11 @@
       </c>
       <c r="J6" s="63"/>
       <c r="K6" s="68"/>
-      <c r="L6" s="96" t="s">
+      <c r="L6" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="96"/>
-      <c r="N6" s="97"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="109"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -15679,11 +15823,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -15718,9 +15862,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -15751,9 +15895,9 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
@@ -15770,19 +15914,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="93">
+      <c r="I10" s="105">
         <f>I5/(SUM(D10:D12))</f>
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="102" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="44"/>
-      <c r="L10" s="101" t="s">
+      <c r="L10" s="110" t="s">
         <v>53</v>
       </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
@@ -15797,8 +15941,8 @@
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="103"/>
       <c r="K11" s="12"/>
       <c r="L11" s="51"/>
       <c r="M11" s="51"/>
@@ -15817,12 +15961,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -15850,9 +15994,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -15891,9 +16035,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -15901,6 +16045,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="J10:J12"/>
     <mergeCell ref="L10:N10"/>
@@ -15911,12 +16061,6 @@
     <mergeCell ref="A2:N3"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="L5:N5"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -15950,8 +16094,8 @@
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15973,55 +16117,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="107" t="str">
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
         <v>BH-42-ethylbenzene</v>
       </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="108"/>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -16051,11 +16195,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -16095,11 +16239,11 @@
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="67"/>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -16142,11 +16286,11 @@
         <v>1.0129999999999999</v>
       </c>
       <c r="K6" s="82"/>
-      <c r="L6" s="98" t="s">
+      <c r="L6" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="99"/>
-      <c r="N6" s="100"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="93"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -16181,11 +16325,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -16220,9 +16364,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -16253,14 +16397,14 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
       <c r="B10" s="79" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="65">
@@ -16272,19 +16416,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="93">
+      <c r="I10" s="105">
         <f>I5/(SUM(D10:D12))</f>
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="102" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="80"/>
-      <c r="L10" s="101" t="s">
-        <v>71</v>
-      </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="L10" s="110" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
@@ -16295,12 +16439,12 @@
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="103"/>
       <c r="K11" s="31"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
-      <c r="N11" s="106"/>
+      <c r="L11" s="114"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="115"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
@@ -16315,12 +16459,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -16348,9 +16492,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -16389,9 +16533,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -16399,23 +16543,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L12:N12"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A2:N3"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -16449,8 +16593,8 @@
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16472,55 +16616,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="107" t="str">
+      <c r="E1" s="86" t="str">
         <f ca="1">Settings!A7&amp;"-"&amp;MID(CELL("filename",B1),FIND("]",CELL("filename",B1))+1,256)</f>
         <v>BH-43-butanol</v>
       </c>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="114" t="s">
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="108" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" s="108"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="87" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
     </row>
     <row r="3" spans="1:14" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="A3" s="101"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="35"/>
@@ -16550,11 +16694,11 @@
       <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="112" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="95"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40">
@@ -16594,11 +16738,11 @@
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="67"/>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="110"/>
-      <c r="N5" s="111"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39">
@@ -16641,11 +16785,11 @@
         <v>1.0129999999999999</v>
       </c>
       <c r="K6" s="82"/>
-      <c r="L6" s="98" t="s">
+      <c r="L6" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="99"/>
-      <c r="N6" s="100"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="93"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="38">
@@ -16680,11 +16824,11 @@
       </c>
       <c r="J7" s="72"/>
       <c r="K7" s="69"/>
-      <c r="L7" s="98" t="s">
+      <c r="L7" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="100"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
@@ -16719,9 +16863,9 @@
       </c>
       <c r="J8" s="73"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="115"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -16752,14 +16896,14 @@
       </c>
       <c r="J9" s="74"/>
       <c r="K9" s="71"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="100"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37"/>
       <c r="B10" s="84" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="65">
@@ -16771,19 +16915,19 @@
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="93">
+      <c r="I10" s="105">
         <f>I5/(SUM(D10:D12))</f>
         <v>0.5</v>
       </c>
-      <c r="J10" s="90" t="s">
+      <c r="J10" s="102" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="80"/>
-      <c r="L10" s="101" t="s">
-        <v>70</v>
-      </c>
-      <c r="M10" s="101"/>
-      <c r="N10" s="102"/>
+      <c r="L10" s="110" t="s">
+        <v>68</v>
+      </c>
+      <c r="M10" s="110"/>
+      <c r="N10" s="111"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
@@ -16794,12 +16938,12 @@
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="91"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="103"/>
       <c r="K11" s="31"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
-      <c r="N11" s="106"/>
+      <c r="L11" s="114"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="115"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
@@ -16814,12 +16958,12 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="92"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="104"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="104"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="113"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
@@ -16847,9 +16991,9 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="88"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
@@ -16888,9 +17032,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="86"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="L16" s="11"/>
@@ -16898,23 +17042,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L12:N12"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A2:N3"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>

</xml_diff>